<commit_message>
added schematic, updated BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quantumhti.sharepoint.com/sites/company/Shared Documents/Quantum Integration/Engineering/Quantum Hardware/DIY Kits/Q-PCB-004/Motor Servo Driver Rev G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{529792D7-A2A6-7348-A0D5-86E785AC7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4D06537-E8D3-B74D-98FC-8323350296EE}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{529792D7-A2A6-7348-A0D5-86E785AC7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5613E193-ACFB-DC4D-9D97-8A0686150C51}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14640" windowWidth="25600" windowHeight="14160" xr2:uid="{B448305C-E8CB-C242-9019-B3A935BA1718}"/>
+    <workbookView xWindow="3620" yWindow="1000" windowWidth="25600" windowHeight="14160" xr2:uid="{B448305C-E8CB-C242-9019-B3A935BA1718}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Header</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>GDS</t>
+  </si>
+  <si>
+    <t>200m</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>E3,5-8</t>
+  </si>
+  <si>
+    <t>H: 12mm, 50V</t>
   </si>
 </sst>
 </file>
@@ -601,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38DB0BD5-94FF-6441-8936-80E17C8BDAE3}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -942,6 +954,9 @@
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D14" s="1">
         <v>4</v>
       </c>
@@ -999,6 +1014,32 @@
       </c>
       <c r="I16" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1018,27 +1059,14 @@
     <hyperlink ref="I15" r:id="rId13" xr:uid="{85C56B4C-1190-6E4A-A9A8-A9D724E3108E}"/>
     <hyperlink ref="I14" r:id="rId14" display="https://www.amazon.com/Resistor-Ltvystore-Fixed-Assortment-0-25W/dp/B07G4YJCNC/ref=sr_1_1_sspa?dchild=1&amp;keywords=resistor+1206&amp;qid=1625619256&amp;sr=8-1-spons&amp;psc=1&amp;smid=ACRAF3O0AXJNI&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzUUg0TlZRWEVQUjhSJmVuY3J5cHRlZElkPUEwMDAzMzE1MVhLVFc0S1ZDMEJZSyZlbmNyeXB0ZWRBZElkPUEwNTQ5Nzk4Nkg2WDlSTzVZUDZSJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{DBC8A2FF-0231-9646-A40A-E558DDFEAA28}"/>
     <hyperlink ref="I13" r:id="rId15" display="https://www.amazon.com/LARSEBEI-10Types-transistors-Assortment-Including/dp/B08QD9CKHM/ref=sr_1_1_sspa?dchild=1&amp;keywords=p+channel+mosfet&amp;qid=1625619278&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyM002WEc4T0IwMVYzJmVuY3J5cHRlZElkPUEwNzY5NjE4MzFSTzJIVVZNOVRSQiZlbmNyeXB0ZWRBZElkPUEwMzQwMzg4RUQySzJYMlVBWlZJJndpZGdldE5hbWU9c3BfYXRmJmFjdGlvbj1jbGlja1JlZGlyZWN0JmRvTm90TG9nQ2xpY2s9dHJ1ZQ==" xr:uid="{B5A28FCC-ABED-B140-9EC2-D58850740B3D}"/>
+    <hyperlink ref="I17" r:id="rId16" xr:uid="{E50D7573-FA63-7A4C-AEDB-40C8763C2031}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D595B56E1980314DA4E383B61D36AA9D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f22e5b04d01c1caa839da4a9af726b7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="97031774-c0c7-48a9-a8e1-3722ddd0f879" xmlns:ns3="a32bd177-85eb-4316-9671-26122bedec74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fea236e577cee3a72401322f0e2f6618" ns2:_="" ns3:_="">
     <xsd:import namespace="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
@@ -1261,32 +1289,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5C9FE4-AA70-4C3D-8985-38F88B112BAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56C34763-A3F9-46A5-9676-3A0DAE10C423}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{054FFDFF-CF3D-4DFA-9625-C3D55A99D2C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1303,4 +1321,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56C34763-A3F9-46A5-9676-3A0DAE10C423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC5C9FE4-AA70-4C3D-8985-38F88B112BAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
+    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>